<commit_message>
[ADD] Tabelas Download eixo 3
</commit_message>
<xml_diff>
--- a/data/csv/mercado/atividades_relacionadas/NECCULT - 2018 - ATLAS - Eixo 2 - Síntese V11.xlsx
+++ b/data/csv/mercado/atividades_relacionadas/NECCULT - 2018 - ATLAS - Eixo 2 - Síntese V11.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suporte\Documents\Sínteses Atlas\Eixo 2 - Ocupacional - Atividades Relacionadas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suporte\Google Drive\Atlas\Dados\Sínteses para download\Eixo 2 - Ocupacional - Ativ. Relacionadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Tabelas" sheetId="1" r:id="rId1"/>
@@ -30,10 +30,10 @@
     <t>C4</t>
   </si>
   <si>
-    <t>Tabela 1 - Evolução do Índice de Concentração C4 do Total de Rendimentos dos das Atividades Relacionadas por UF entre 2007 e 2014</t>
+    <t>V8 - Razão de Concentração da Massa de Rendimentos do Trabalho (C4)</t>
   </si>
   <si>
-    <t>V8 - Razão de Concentração da Massa de Rendimentos do Trabalho (C4)</t>
+    <t>Tabela 1 - Evolução do Índice de Concentração C4 do Total de Rendimentos dos das Atividades Relacionadas por UF entre 2007 e 2015</t>
   </si>
 </sst>
 </file>
@@ -413,15 +413,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -438,7 +438,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -469,15 +469,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -503,19 +503,19 @@
         <v>2009</v>
       </c>
       <c r="E2" s="1">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="F2" s="1">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="G2" s="1">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="H2" s="1">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="I2" s="1">
-        <v>2014</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -523,25 +523,25 @@
         <v>0</v>
       </c>
       <c r="B3" s="2">
-        <v>0.6605868806284162</v>
+        <v>0.64941377886383655</v>
       </c>
       <c r="C3" s="2">
-        <v>0.63851606787772486</v>
+        <v>0.66888748756939687</v>
       </c>
       <c r="D3" s="2">
-        <v>0.61345213747907401</v>
+        <v>0.63269189492511901</v>
       </c>
       <c r="E3" s="2">
-        <v>0.61016942362388005</v>
+        <v>0.64001049055683878</v>
       </c>
       <c r="F3" s="2">
-        <v>0.63396051099017747</v>
+        <v>0.62574470603802668</v>
       </c>
       <c r="G3" s="2">
-        <v>0.6263904640935678</v>
+        <v>0.64228437110822345</v>
       </c>
       <c r="H3" s="2">
-        <v>0.66578942675602404</v>
+        <v>0.64233690451414227</v>
       </c>
       <c r="I3" s="2">
         <v>0.63916489448919878</v>

</xml_diff>